<commit_message>
clean code & refactoring fix : validasi nomor kendaraan
</commit_message>
<xml_diff>
--- a/database/Data_Parking.xlsx
+++ b/database/Data_Parking.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J56"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3213,6 +3213,156 @@
         </is>
       </c>
     </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>QIPZ5P2BG6MW</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>D 5034 YAW</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Motor</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>2025-01-13 17:00:18</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>2025-01-13 17:00:57</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>0.0 jam 0.0 menit 39.717722 detik</t>
+        </is>
+      </c>
+      <c r="G57" t="n">
+        <v>2000</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>Reza Ramdan Permana</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>./capture/masuk/QIPZ5P2BG6MW.png</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>./capture/keluar/QIPZ5P2BG6MW.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>8E3FKYN6OBLV</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>D 5430 BAH</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Mobil</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>2025-01-13 17:14:36</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>2025-01-13 17:15:17</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>00:00:41</t>
+        </is>
+      </c>
+      <c r="G58" t="n">
+        <v>4000</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Reza Ramdan Permana</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>./capture/masuk/8E3FKYN6OBLV.png</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>./capture/keluar/8E3FKYN6OBLV.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>3GH15R2GL0YE</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>D 6405 HWK</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Motor</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>2025-01-13 17:21:11</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>2025-01-13 17:22:06</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>00:00:55</t>
+        </is>
+      </c>
+      <c r="G59" t="n">
+        <v>2000</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>Reza Ramdan Permana</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>./capture/masuk/3GH15R2GL0YE.png</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>./capture/keluar/3GH15R2GL0YE.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
no 4 sudah btul tinggal mengatur tanggal berapa saja yang mau di ambil
</commit_message>
<xml_diff>
--- a/database/Data_Parking.xlsx
+++ b/database/Data_Parking.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,43 +493,39 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>RCCF584T2B12</t>
+          <t>NJ9E1D0UMB22</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Y 3249 ASD</t>
+          <t>Y 0313 HAS</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t> </t>
+          <t>Motor</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2025-01-31 16:06:35</t>
+          <t>2025-01-31 21:09:22</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t> </t>
+          <t>2025-01-31 21:09:47</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
+          <t>00:00:25</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="H2" t="n">
+        <v>5000</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -538,65 +534,118 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>./capture/masuk/RCCF584T2B12.png</t>
+          <t>./capture/masuk/NJ9E1D0UMB22.png</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t> </t>
+          <t>./capture/keluar/NJ9E1D0UMB22.png</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>IULMD53YWRNI</t>
+          <t>SN12XKBEG18L</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>A 4203 ASD</t>
+          <t>D 4230 ASQ</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>Mobil</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-01-31 21:10:39</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2025-01-31 21:11:58</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>00:01:19</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>4000</v>
+      </c>
+      <c r="H3" t="n">
+        <v>60000</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Reza Ramdan Permana</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>./capture/masuk/SN12XKBEG18L.png</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>./capture/keluar/SN12XKBEG18L.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>58O0J9BUUNER</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>D 9530 JFD</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>Motor</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2025-01-31 16:09:37</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2025-01-31 16:10:17</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>00:00:40</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-01-31 21:15:34</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2025-01-31 21:16:09</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>00:00:35</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
         <v>2000</v>
       </c>
-      <c r="H3" t="n">
-        <v>5999</v>
-      </c>
-      <c r="I3" t="inlineStr">
+      <c r="H4" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>Reza Ramdan Permana</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>./capture/masuk/IULMD53YWRNI.png</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>./capture/keluar/IULMD53YWRNI.png</t>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>./capture/masuk/58O0J9BUUNER.png</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>./capture/keluar/58O0J9BUUNER.png</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix : Laporan Keuangan Parkir Selesai. Fitur : Membuat fitur delete data parkir
</commit_message>
<xml_diff>
--- a/database/Data_Parking.xlsx
+++ b/database/Data_Parking.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -619,33 +619,249 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-01-31 21:16:09</t>
+          <t>2025-02-03 17:46:10</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>00:00:35</t>
+          <t>68:30:36</t>
         </is>
       </c>
       <c r="G4" t="n">
+        <v>138000</v>
+      </c>
+      <c r="H4" t="n">
+        <v>500000</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Reza Ramdan Permana</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>./capture/masuk/58O0J9BUUNER.png</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>./capture/keluar/58O0J9BUUNER.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>E27U7I7WBKVU</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>D 3420 ASW</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Motor</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2025-02-03 16:14:03</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2025-02-03 16:15:49</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>00:01:46</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
         <v>2000</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H5" t="n">
         <v>5000</v>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>Reza Ramdan Permana</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>./capture/masuk/58O0J9BUUNER.png</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>./capture/keluar/58O0J9BUUNER.png</t>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>./capture/masuk/E27U7I7WBKVU.png</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>./capture/keluar/E27U7I7WBKVU.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Y5SWQW4LEWJW</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>B 4203 UYS</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Mobil</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2025-02-03 16:18:24</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2025-02-03 16:19:00</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>00:00:36</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>4000</v>
+      </c>
+      <c r="H6" t="n">
+        <v>60000</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Reza Ramdan Permana</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>./capture/masuk/Y5SWQW4LEWJW.png</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>./capture/keluar/Y5SWQW4LEWJW.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6CFX94LN9BM1</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>D 3240 CUY</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Motor</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2025-02-03 17:40:06</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2025-02-03 17:44:07</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>00:04:01</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>2000</v>
+      </c>
+      <c r="H7" t="n">
+        <v>50000</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Reza Ramdan Permana</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>./capture/masuk/6CFX94LN9BM1.png</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>./capture/keluar/6CFX94LN9BM1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>PCARMF5WXU87</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>C 3402 DFA</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2025-02-03 17:40:57</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Reza Ramdan Permana</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>./capture/masuk/PCARMF5WXU87.png</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fitur : hapus data parkir selesai
</commit_message>
<xml_diff>
--- a/database/Data_Parking.xlsx
+++ b/database/Data_Parking.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -546,39 +546,39 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SN12XKBEG18L</t>
+          <t>58O0J9BUUNER</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>D 4230 ASQ</t>
+          <t>D 9530 JFD</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Mobil</t>
+          <t>Motor</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2025-01-31 21:10:39</t>
+          <t>2025-01-31 21:15:34</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-01-31 21:11:58</t>
+          <t>2025-02-03 17:46:10</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>00:01:19</t>
+          <t>68:30:36</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>4000</v>
+        <v>138000</v>
       </c>
       <c r="H3" t="n">
-        <v>60000</v>
+        <v>500000</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -587,24 +587,24 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>./capture/masuk/SN12XKBEG18L.png</t>
+          <t>./capture/masuk/58O0J9BUUNER.png</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>./capture/keluar/SN12XKBEG18L.png</t>
+          <t>./capture/keluar/58O0J9BUUNER.png</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>58O0J9BUUNER</t>
+          <t>E27U7I7WBKVU</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>D 9530 JFD</t>
+          <t>D 3420 ASW</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -614,24 +614,24 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2025-01-31 21:15:34</t>
+          <t>2025-02-03 16:14:03</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-02-03 17:46:10</t>
+          <t>2025-02-03 16:15:49</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>68:30:36</t>
+          <t>00:01:46</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>138000</v>
+        <v>2000</v>
       </c>
       <c r="H4" t="n">
-        <v>500000</v>
+        <v>5000</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -640,51 +640,51 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>./capture/masuk/58O0J9BUUNER.png</t>
+          <t>./capture/masuk/E27U7I7WBKVU.png</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>./capture/keluar/58O0J9BUUNER.png</t>
+          <t>./capture/keluar/E27U7I7WBKVU.png</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>E27U7I7WBKVU</t>
+          <t>Y5SWQW4LEWJW</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>D 3420 ASW</t>
+          <t>B 4203 UYS</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Motor</t>
+          <t>Mobil</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2025-02-03 16:14:03</t>
+          <t>2025-02-03 16:18:24</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-02-03 16:15:49</t>
+          <t>2025-02-03 16:19:00</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>00:01:46</t>
+          <t>00:00:36</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="H5" t="n">
-        <v>5000</v>
+        <v>60000</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -693,51 +693,51 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>./capture/masuk/E27U7I7WBKVU.png</t>
+          <t>./capture/masuk/Y5SWQW4LEWJW.png</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>./capture/keluar/E27U7I7WBKVU.png</t>
+          <t>./capture/keluar/Y5SWQW4LEWJW.png</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Y5SWQW4LEWJW</t>
+          <t>6CFX94LN9BM1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>B 4203 UYS</t>
+          <t>D 3240 CUY</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Mobil</t>
+          <t>Motor</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2025-02-03 16:18:24</t>
+          <t>2025-02-03 17:40:06</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-02-03 16:19:00</t>
+          <t>2025-02-03 17:44:07</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>00:00:36</t>
+          <t>00:04:01</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="H6" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -746,51 +746,55 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>./capture/masuk/Y5SWQW4LEWJW.png</t>
+          <t>./capture/masuk/6CFX94LN9BM1.png</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>./capture/keluar/Y5SWQW4LEWJW.png</t>
+          <t>./capture/keluar/6CFX94LN9BM1.png</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>6CFX94LN9BM1</t>
+          <t>TXDSWY5EZFB6</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>D 3240 CUY</t>
+          <t>D 0423 JS</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Motor</t>
+          <t> </t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2025-02-03 17:40:06</t>
+          <t>2025-02-03 18:56:00</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-02-03 17:44:07</t>
+          <t> </t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>00:04:01</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
-        <v>2000</v>
-      </c>
-      <c r="H7" t="n">
-        <v>50000</v>
+          <t> </t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -799,67 +803,10 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>./capture/masuk/6CFX94LN9BM1.png</t>
+          <t>./capture/masuk/TXDSWY5EZFB6.png</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
-        <is>
-          <t>./capture/keluar/6CFX94LN9BM1.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>PCARMF5WXU87</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>C 3402 DFA</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>2025-02-03 17:40:57</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>Reza Ramdan Permana</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>./capture/masuk/PCARMF5WXU87.png</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
         <is>
           <t> </t>
         </is>

</xml_diff>